<commit_message>
[#134279773] Importação de usuários aceita informação de turma
</commit_message>
<xml_diff>
--- a/public/modelo-importacao.xlsx
+++ b/public/modelo-importacao.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="modelo-importacao" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t xml:space="preserve">Nome</t>
   </si>
@@ -49,6 +49,9 @@
     <t xml:space="preserve">Instituição</t>
   </si>
   <si>
+    <t xml:space="preserve">Turma</t>
+  </si>
+  <si>
     <t xml:space="preserve">Elenora W. Conners</t>
   </si>
   <si>
@@ -73,6 +76,9 @@
     <t xml:space="preserve">UFC</t>
   </si>
   <si>
+    <t xml:space="preserve">Turma A</t>
+  </si>
+  <si>
     <t xml:space="preserve">Erick Ribeiro Rodrigues</t>
   </si>
   <si>
@@ -83,6 +89,9 @@
   </si>
   <si>
     <t xml:space="preserve">Travessa Visconde de Cachoeira, 112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turma B</t>
   </si>
   <si>
     <t xml:space="preserve">Luana Barbosa Dias</t>
@@ -188,24 +197,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5867346938776"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.1836734693878"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.58673469387755"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -236,92 +244,101 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>61812736700</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>14837238520</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>30282151791</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merge com servidores de produção
</commit_message>
<xml_diff>
--- a/public/modelo-importacao.xlsx
+++ b/public/modelo-importacao.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="modelo-importacao" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t xml:space="preserve">Nome</t>
   </si>
@@ -52,16 +52,16 @@
     <t xml:space="preserve">Turma</t>
   </si>
   <si>
-    <t xml:space="preserve">Elenora W. Conners</t>
+    <t xml:space="preserve">Fulano Silva</t>
   </si>
   <si>
     <t xml:space="preserve">F</t>
   </si>
   <si>
-    <t xml:space="preserve">elenorawconners@mail1.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avenida Mercedes Martins Vieira, 351</t>
+    <t xml:space="preserve">fulano@email.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avenida A, 123</t>
   </si>
   <si>
     <t xml:space="preserve">Brasil</t>
@@ -79,28 +79,28 @@
     <t xml:space="preserve">Turma A</t>
   </si>
   <si>
-    <t xml:space="preserve">Erick Ribeiro Rodrigues</t>
+    <t xml:space="preserve">Beltrano Pereira</t>
   </si>
   <si>
     <t xml:space="preserve">M</t>
   </si>
   <si>
-    <t xml:space="preserve">rodrigues@mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Travessa Visconde de Cachoeira, 112</t>
+    <t xml:space="preserve">beltrano@email.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua B, 222</t>
   </si>
   <si>
     <t xml:space="preserve">Turma B</t>
   </si>
   <si>
-    <t xml:space="preserve">Luana Barbosa Dias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">luana@mail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rua C, 963</t>
+    <t xml:space="preserve">Ciclano Soares</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ciclano@email.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua C, 333</t>
   </si>
 </sst>
 </file>
@@ -110,7 +110,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -131,6 +131,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -175,8 +182,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -199,21 +210,22 @@
   </sheetPr>
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.1836734693878"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.58673469387755"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -248,17 +260,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>61812736700</v>
+        <v>11111111111</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="0" t="s">
@@ -280,17 +292,17 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>14837238520</v>
+        <v>22222222222</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E3" s="0" t="s">
@@ -312,17 +324,17 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>30282151791</v>
+        <v>12345678910</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E4" s="0" t="s">
@@ -340,11 +352,19 @@
       <c r="I4" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="J4" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="fulano@email.com"/>
+    <hyperlink ref="D3" r:id="rId2" display="beltrano@email.com"/>
+    <hyperlink ref="D4" r:id="rId3" display="ciclano@email.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>

</xml_diff>